<commit_message>
checkin for interfaces and upgrades
</commit_message>
<xml_diff>
--- a/data/ArcGISDesktop_TC01.xlsx
+++ b/data/ArcGISDesktop_TC01.xlsx
@@ -111,97 +111,97 @@
     <t>Be a Trusted Source of Relevant Information</t>
   </si>
   <si>
+    <t>Get the Answers That Your Organization Is Looking for</t>
+  </si>
+  <si>
+    <t>Powerful Applications</t>
+  </si>
+  <si>
+    <t>ArcMap</t>
+  </si>
+  <si>
+    <t>ArcGIS Pro</t>
+  </si>
+  <si>
+    <t>Key Features</t>
+  </si>
+  <si>
+    <t>Conduct Spatial Analysis</t>
+  </si>
+  <si>
+    <t>Manage Your Data More Efficiently</t>
+  </si>
+  <si>
+    <t>Explore a World of Content</t>
+  </si>
+  <si>
+    <t>Automate Advanced Workflows</t>
+  </si>
+  <si>
+    <t>Easily Create Maps</t>
+  </si>
+  <si>
+    <t>Start Geocoding</t>
+  </si>
+  <si>
+    <t>Access Advanced Imagery</t>
+  </si>
+  <si>
+    <t>Give Your Clients What They Need</t>
+  </si>
+  <si>
+    <t>What's New in ArcGIS</t>
+  </si>
+  <si>
+    <t>Extensions</t>
+  </si>
+  <si>
+    <t>System Requirements</t>
+  </si>
+  <si>
+    <t>Pricing</t>
+  </si>
+  <si>
+    <t>Programs and ELAs</t>
+  </si>
+  <si>
+    <t>What Do I Get with My Free ArcGIS Trial?</t>
+  </si>
+  <si>
+    <t>fName</t>
+  </si>
+  <si>
+    <t>lName</t>
+  </si>
+  <si>
+    <t>emailId</t>
+  </si>
+  <si>
+    <t>ConfirmemailId</t>
+  </si>
+  <si>
+    <t>IndustryDpDwn</t>
+  </si>
+  <si>
+    <t>esri</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>balaji.harinath@htcindia.com</t>
+  </si>
+  <si>
+    <t>Community Planning/Economic Development</t>
+  </si>
+  <si>
+    <t>cmNotify</t>
+  </si>
+  <si>
+    <t>Confirmation Email Sent!</t>
+  </si>
+  <si>
     <t>You Know It Is Science—Everyone Else Can Call It Secret Sauce</t>
-  </si>
-  <si>
-    <t>Get the Answers That Your Organization Is Looking for</t>
-  </si>
-  <si>
-    <t>Powerful Applications</t>
-  </si>
-  <si>
-    <t>ArcMap</t>
-  </si>
-  <si>
-    <t>ArcGIS Pro</t>
-  </si>
-  <si>
-    <t>Key Features</t>
-  </si>
-  <si>
-    <t>Conduct Spatial Analysis</t>
-  </si>
-  <si>
-    <t>Manage Your Data More Efficiently</t>
-  </si>
-  <si>
-    <t>Explore a World of Content</t>
-  </si>
-  <si>
-    <t>Automate Advanced Workflows</t>
-  </si>
-  <si>
-    <t>Easily Create Maps</t>
-  </si>
-  <si>
-    <t>Start Geocoding</t>
-  </si>
-  <si>
-    <t>Access Advanced Imagery</t>
-  </si>
-  <si>
-    <t>Give Your Clients What They Need</t>
-  </si>
-  <si>
-    <t>What's New in ArcGIS</t>
-  </si>
-  <si>
-    <t>Extensions</t>
-  </si>
-  <si>
-    <t>System Requirements</t>
-  </si>
-  <si>
-    <t>Pricing</t>
-  </si>
-  <si>
-    <t>Programs and ELAs</t>
-  </si>
-  <si>
-    <t>What Do I Get with My Free ArcGIS Trial?</t>
-  </si>
-  <si>
-    <t>fName</t>
-  </si>
-  <si>
-    <t>lName</t>
-  </si>
-  <si>
-    <t>emailId</t>
-  </si>
-  <si>
-    <t>ConfirmemailId</t>
-  </si>
-  <si>
-    <t>IndustryDpDwn</t>
-  </si>
-  <si>
-    <t>esri</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>balaji.harinath@htcindia.com</t>
-  </si>
-  <si>
-    <t>Community Planning/Economic Development</t>
-  </si>
-  <si>
-    <t>cmNotify</t>
-  </si>
-  <si>
-    <t>Confirmation Email Sent!</t>
   </si>
 </sst>
 </file>
@@ -554,7 +554,7 @@
   <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -647,22 +647,22 @@
         <v>25</v>
       </c>
       <c r="Z1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA1" t="s">
         <v>50</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>51</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>52</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>53</v>
       </c>
-      <c r="AD1" t="s">
-        <v>54</v>
-      </c>
       <c r="AE1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
@@ -682,82 +682,82 @@
         <v>29</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="V2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="W2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="X2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="Y2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="Y2" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="Z2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD2" t="s">
         <v>57</v>
       </c>
-      <c r="AC2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>58</v>
-      </c>
       <c r="AE2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>